<commit_message>
iterate through * number of blocks
</commit_message>
<xml_diff>
--- a/resources/GG_Links.xlsx
+++ b/resources/GG_Links.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben.Turner\Documents\code\python\ggpy\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157C64CA-7F33-4C05-86C1-10630DF8A2DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D84C3EA-95CC-4CDA-855F-C297006947A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1995" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4515" yWindow="1005" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="master" sheetId="1" r:id="rId1"/>
+    <sheet name="master" sheetId="2" r:id="rId1"/>
+    <sheet name="carousels" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Hero</t>
   </si>
@@ -39,109 +40,163 @@
     <t xml:space="preserve">Browse gifts block 1 </t>
   </si>
   <si>
-    <t>block 1</t>
-  </si>
-  <si>
     <t>Browse gifts block 2</t>
   </si>
   <si>
-    <t>block 2</t>
-  </si>
-  <si>
     <t>Browse gifts block 3</t>
   </si>
   <si>
-    <t>block 3</t>
-  </si>
-  <si>
     <t>Browse gifts block 4</t>
   </si>
   <si>
-    <t>block 4</t>
-  </si>
-  <si>
     <t>Popular categiries left</t>
   </si>
   <si>
-    <t>block 5</t>
-  </si>
-  <si>
     <t>Popular categiries right</t>
   </si>
   <si>
-    <t>block 6</t>
-  </si>
-  <si>
     <t>Gifts for under £40 cta</t>
   </si>
   <si>
-    <t>block 7</t>
-  </si>
-  <si>
-    <t>Gifts for under £40 block 1</t>
-  </si>
-  <si>
-    <t>block 8</t>
-  </si>
-  <si>
-    <t>Gifts for under £40 block 2</t>
-  </si>
-  <si>
-    <t>block 9</t>
-  </si>
-  <si>
     <t>Gifts for under £40 block 3</t>
   </si>
   <si>
-    <t>block 10</t>
-  </si>
-  <si>
     <t>Gifts for under £40 block 4</t>
   </si>
   <si>
-    <t>block 11</t>
-  </si>
-  <si>
     <t>Inspiration Block 1</t>
   </si>
   <si>
-    <t>block 12</t>
-  </si>
-  <si>
     <t>Inspiration Block 2</t>
   </si>
   <si>
-    <t>block 13</t>
-  </si>
-  <si>
     <t>Inspiration Block 3</t>
   </si>
   <si>
-    <t>block 14</t>
-  </si>
-  <si>
     <t>Inspiration Block 4</t>
   </si>
   <si>
-    <t>block 15</t>
-  </si>
-  <si>
-    <t>Blog block 1</t>
-  </si>
-  <si>
-    <t>block 16</t>
-  </si>
-  <si>
-    <t>Blog block 2</t>
-  </si>
-  <si>
-    <t>block 17</t>
-  </si>
-  <si>
-    <t>Blog block 3</t>
-  </si>
-  <si>
-    <t>block 18</t>
+    <t>Browse gifts block 5</t>
+  </si>
+  <si>
+    <t>Browse gifts block 6</t>
+  </si>
+  <si>
+    <t>cta</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>bg1</t>
+  </si>
+  <si>
+    <t>bg2</t>
+  </si>
+  <si>
+    <t>bg3</t>
+  </si>
+  <si>
+    <t>bg4</t>
+  </si>
+  <si>
+    <t>bg5</t>
+  </si>
+  <si>
+    <t>bg6</t>
+  </si>
+  <si>
+    <t>gfu401</t>
+  </si>
+  <si>
+    <t>gfu402</t>
+  </si>
+  <si>
+    <t>gfu403</t>
+  </si>
+  <si>
+    <t>gfu404</t>
+  </si>
+  <si>
+    <t>i1</t>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>i3</t>
+  </si>
+  <si>
+    <t>i4</t>
+  </si>
+  <si>
+    <t>Browse gifts block 7</t>
+  </si>
+  <si>
+    <t>bg7</t>
+  </si>
+  <si>
+    <t>Browse gifts block 8</t>
+  </si>
+  <si>
+    <t>bg8</t>
+  </si>
+  <si>
+    <t>Gifts for under £40 block 5</t>
+  </si>
+  <si>
+    <t>gfu405</t>
+  </si>
+  <si>
+    <t>Gifts for under £40 block 6</t>
+  </si>
+  <si>
+    <t>Gifts for under £40 block 7</t>
+  </si>
+  <si>
+    <t>Inspiration Block 5</t>
+  </si>
+  <si>
+    <t>i5</t>
+  </si>
+  <si>
+    <t>Inspiration Block 6</t>
+  </si>
+  <si>
+    <t>i6</t>
+  </si>
+  <si>
+    <t>Inspiration Block 7</t>
+  </si>
+  <si>
+    <t>i7</t>
+  </si>
+  <si>
+    <t>Inspiration Block 8</t>
+  </si>
+  <si>
+    <t>i8</t>
+  </si>
+  <si>
+    <t>Blog 1</t>
+  </si>
+  <si>
+    <t>Blog 2</t>
+  </si>
+  <si>
+    <t>Blog 3</t>
+  </si>
+  <si>
+    <t>bb1</t>
+  </si>
+  <si>
+    <t>bb2</t>
+  </si>
+  <si>
+    <t>bb3</t>
   </si>
 </sst>
 </file>
@@ -511,11 +566,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33B44AA-D287-4733-A773-F815C7718588}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,18 +631,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -545,116 +650,116 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>33</v>
@@ -662,18 +767,58 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add gifts under 40 module
</commit_message>
<xml_diff>
--- a/resources/GG_Links.xlsx
+++ b/resources/GG_Links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben.Turner\Documents\code\python\ggpy\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D84C3EA-95CC-4CDA-855F-C297006947A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC4ACE5-0647-4E1F-9EE7-77F128A7224B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="1005" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29190" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Hero</t>
   </si>
@@ -133,30 +133,6 @@
     <t>i4</t>
   </si>
   <si>
-    <t>Browse gifts block 7</t>
-  </si>
-  <si>
-    <t>bg7</t>
-  </si>
-  <si>
-    <t>Browse gifts block 8</t>
-  </si>
-  <si>
-    <t>bg8</t>
-  </si>
-  <si>
-    <t>Gifts for under £40 block 5</t>
-  </si>
-  <si>
-    <t>gfu405</t>
-  </si>
-  <si>
-    <t>Gifts for under £40 block 6</t>
-  </si>
-  <si>
-    <t>Gifts for under £40 block 7</t>
-  </si>
-  <si>
     <t>Inspiration Block 5</t>
   </si>
   <si>
@@ -197,6 +173,39 @@
   </si>
   <si>
     <t>bb3</t>
+  </si>
+  <si>
+    <t>Gifts for under £40 block 1</t>
+  </si>
+  <si>
+    <t>Gifts for under £40 block 2</t>
+  </si>
+  <si>
+    <t>Gifts for under £20 block 1</t>
+  </si>
+  <si>
+    <t>Gifts for under £20 block 2</t>
+  </si>
+  <si>
+    <t>Gifts for under £20 block 3</t>
+  </si>
+  <si>
+    <t>Gifts for under £20 block 4</t>
+  </si>
+  <si>
+    <t>gfu201</t>
+  </si>
+  <si>
+    <t>gfu202</t>
+  </si>
+  <si>
+    <t>gfu203</t>
+  </si>
+  <si>
+    <t>gfu204</t>
+  </si>
+  <si>
+    <t>Gifts for under £20 cta</t>
   </si>
 </sst>
 </file>
@@ -567,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33B44AA-D287-4733-A773-F815C7718588}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +597,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
@@ -596,17 +605,25 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -617,10 +634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,146 +696,154 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>